<commit_message>
new register graph sheet
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_graph.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2880"/>
   </bookViews>
   <sheets>
     <sheet name="final graphs" sheetId="2" r:id="rId1"/>
@@ -1528,16 +1528,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1799,20 +1793,53 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1829,52 +1856,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1973,7 +1973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{604CEEB8-2F5D-48F8-9652-A642EC7F9D4D}" type="CELLRANGE">
+                    <a:fld id="{0052D5B5-5B55-451D-ABEE-6330E1BBF2A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2007,7 +2007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{724EFD36-362E-40BA-9C37-031CD61BAA83}" type="CELLRANGE">
+                    <a:fld id="{8A440E0E-BA2D-45EB-94A9-BE15EE315B09}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2039,7 +2039,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FAB5812-2C99-4E50-B676-F460871D3D4A}" type="CELLRANGE">
+                    <a:fld id="{3FFC0300-F09F-49AF-860D-C1D0A7E22B54}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2295,11 +2295,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1120201744"/>
-        <c:axId val="-917197888"/>
+        <c:axId val="-1246289904"/>
+        <c:axId val="-1246287184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1120201744"/>
+        <c:axId val="-1246289904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2322,7 +2322,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-917197888"/>
+        <c:crossAx val="-1246287184"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2330,7 +2330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-917197888"/>
+        <c:axId val="-1246287184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2418,7 +2418,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-917197888"/>
+        <c:crossAx val="-1246287184"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2595,7 +2595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF512D8A-DA45-4F50-A455-504983DEF090}" type="CELLRANGE">
+                    <a:fld id="{1F9BA23B-DC78-4201-8F88-9D07FD1BFF4E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2635,7 +2635,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C24CF491-9A29-41BF-B3B2-8E592E90D762}" type="CELLRANGE">
+                    <a:fld id="{2DA7EF24-CAB8-4741-8779-828EB8D7CC74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2675,7 +2675,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{903BDF6B-1D4C-485E-A507-7D3BC86C2485}" type="CELLRANGE">
+                    <a:fld id="{B7E54EF7-F340-4DC6-A231-3EC6B10B3BCC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2870,8 +2870,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-916656384"/>
-        <c:axId val="-916661280"/>
+        <c:axId val="-1268461888"/>
+        <c:axId val="-1268456992"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -2952,11 +2952,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-916659104"/>
-        <c:axId val="-916660192"/>
+        <c:axId val="-1268458624"/>
+        <c:axId val="-1268468960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-916656384"/>
+        <c:axId val="-1268461888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2979,7 +2979,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916661280"/>
+        <c:crossAx val="-1268456992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2987,7 +2987,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-916661280"/>
+        <c:axId val="-1268456992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3086,12 +3086,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916656384"/>
+        <c:crossAx val="-1268461888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-916660192"/>
+        <c:axId val="-1268468960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3101,12 +3101,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-916659104"/>
+        <c:crossAx val="-1268458624"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-916659104"/>
+        <c:axId val="-1268458624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3134,7 +3134,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916660192"/>
+        <c:crossAx val="-1268468960"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3242,13 +3242,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79D010D1-850F-4669-8C8B-EB22410D9375}" type="CELLRANGE">
+                    <a:fld id="{E553A38B-C548-4787-AAE8-77E4180C643E}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -3266,7 +3265,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -3275,13 +3273,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40739843-BB1C-44F9-9334-F90D5C75EF7E}" type="CELLRANGE">
+                    <a:fld id="{46BFB2EF-DC90-4686-A43F-FE26CD9ECE76}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -3299,7 +3296,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -3308,13 +3304,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{224EF9EB-A47D-4C23-BA54-D51E3FC9621A}" type="CELLRANGE">
+                    <a:fld id="{90276E99-605A-4793-8F25-EEFBBE711ED4}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -3332,7 +3327,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -3371,7 +3365,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
@@ -3750,11 +3743,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-916656928"/>
-        <c:axId val="-916652576"/>
+        <c:axId val="-1268462976"/>
+        <c:axId val="-1268460800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-916656928"/>
+        <c:axId val="-1268462976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3777,7 +3770,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916652576"/>
+        <c:crossAx val="-1268460800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3785,7 +3778,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-916652576"/>
+        <c:axId val="-1268460800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3846,7 +3839,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916652576"/>
+        <c:crossAx val="-1268460800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3950,7 +3943,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F8384D7-65B5-486D-BF09-F029A6D1CF6F}" type="CELLRANGE">
+                    <a:fld id="{141D8777-F402-4C07-9FE5-3171796509D4}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -3982,7 +3975,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A97C198C-F0C7-4856-8AE9-39E0E7157CC5}" type="CELLRANGE">
+                    <a:fld id="{7C77AD75-705D-4F48-9361-640635B4CC6F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -4014,7 +4007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAF7A8BA-A9B4-4769-BF7C-6CE5F522AA32}" type="CELLRANGE">
+                    <a:fld id="{0F597E51-A072-4EBA-8C1E-5D6E9C270544}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -4207,11 +4200,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-915684912"/>
-        <c:axId val="-915684368"/>
+        <c:axId val="-1268456448"/>
+        <c:axId val="-1268458080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-915684912"/>
+        <c:axId val="-1268456448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4234,7 +4227,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-915684368"/>
+        <c:crossAx val="-1268458080"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4242,7 +4235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-915684368"/>
+        <c:axId val="-1268458080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4330,7 +4323,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-915684368"/>
+        <c:crossAx val="-1268458080"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4558,7 +4551,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{754C6A42-617F-4159-999C-4899F28156E0}" type="CELLRANGE">
+                    <a:fld id="{BDD5E12B-66A9-4330-A270-D5ABDC97E4B5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -4590,7 +4583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C722963A-3437-4D73-996A-16F48886D151}" type="CELLRANGE">
+                    <a:fld id="{F82BC5D8-3420-4522-8FDB-1BB0BE453B71}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -4876,7 +4869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{289A5DAA-0EE1-42F9-9ED7-7B786AB2B610}" type="CELLRANGE">
+                    <a:fld id="{3FC13F79-F3D1-4464-AE17-2148F35D89E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -4911,7 +4904,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{355A7D4F-23A3-4E76-B940-B145EBBF72EE}" type="CELLRANGE">
+                    <a:fld id="{DF7836F1-D22B-4E3A-81D8-29085F789632}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -4944,7 +4937,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17C9BF5D-1F51-4703-A4A5-145EFB80B6FE}" type="CELLRANGE">
+                    <a:fld id="{BC694BD7-2541-42B4-AF86-0C0528AC5B84}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -5215,8 +5208,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-915680016"/>
-        <c:axId val="-915685456"/>
+        <c:axId val="-1268455904"/>
+        <c:axId val="-1268464608"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -5301,11 +5294,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-915678384"/>
-        <c:axId val="-915679472"/>
+        <c:axId val="-1268468416"/>
+        <c:axId val="-1268467872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-915680016"/>
+        <c:axId val="-1268455904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5332,7 +5325,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-915685456"/>
+        <c:crossAx val="-1268464608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5340,7 +5333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-915685456"/>
+        <c:axId val="-1268464608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5439,12 +5432,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-915680016"/>
+        <c:crossAx val="-1268455904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-915679472"/>
+        <c:axId val="-1268467872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5454,12 +5447,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-915678384"/>
+        <c:crossAx val="-1268468416"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-915678384"/>
+        <c:axId val="-1268468416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5487,7 +5480,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-915679472"/>
+        <c:crossAx val="-1268467872"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5695,7 +5688,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B907D7B0-F3CD-4656-993E-7533DBDA047C}" type="CELLRANGE">
+                    <a:fld id="{3B4B7466-F4A9-46A8-9062-7612436F26FE}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -5727,7 +5720,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E94A33EF-D661-4406-8634-1AFB8C328948}" type="CELLRANGE">
+                    <a:fld id="{42D8EA63-5C31-449A-8F0C-8E576A98DADE}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6013,7 +6006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC8D831B-5CB1-42BA-9492-7711B030AD59}" type="CELLRANGE">
+                    <a:fld id="{EA014BAC-7126-464F-BB0C-0B45068A7AD8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6048,7 +6041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B17ED3E-9035-4814-930E-0D263FC05FC5}" type="CELLRANGE">
+                    <a:fld id="{8C7E1DEB-76A5-4867-82DE-98C52F2E2D71}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6081,7 +6074,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B348F8F-D5D1-4E11-BDCA-72590ACFE62C}" type="CELLRANGE">
+                    <a:fld id="{AB3A27C1-3C54-4A91-A733-A3DC01696C09}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6339,11 +6332,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-917198976"/>
-        <c:axId val="-917200608"/>
+        <c:axId val="-1308274992"/>
+        <c:axId val="-1268792016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-917198976"/>
+        <c:axId val="-1308274992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6366,7 +6359,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-917200608"/>
+        <c:crossAx val="-1268792016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6374,7 +6367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-917200608"/>
+        <c:axId val="-1268792016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6466,7 +6459,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-917200608"/>
+        <c:crossAx val="-1268792016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6608,7 +6601,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40BB5A11-3D6E-48F9-B4CD-21E83B660020}" type="CELLRANGE">
+                    <a:fld id="{BEAA11FD-5A5E-4AB1-9206-E926C36A00E6}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6638,7 +6631,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{280C6305-B8E1-4CE5-A55B-33079B1112A4}" type="CELLRANGE">
+                    <a:fld id="{F3FD0C48-C558-44CF-8D82-220DEECDC195}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -6892,11 +6885,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-917198432"/>
-        <c:axId val="-917197344"/>
+        <c:axId val="-1268789296"/>
+        <c:axId val="-1268795280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-917198432"/>
+        <c:axId val="-1268789296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6922,7 +6915,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-917197344"/>
+        <c:crossAx val="-1268795280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6930,7 +6923,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-917197344"/>
+        <c:axId val="-1268795280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -7021,7 +7014,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-917197344"/>
+        <c:crossAx val="-1268795280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7202,7 +7195,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B73742C-C10A-4992-AB41-8F17BF9E0C37}" type="CELLRANGE">
+                    <a:fld id="{CBE15FD2-D3BC-4198-85D5-B529D52A34AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -7242,7 +7235,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69BC29D5-F70C-46AC-8C3C-AE11CB886DFE}" type="CELLRANGE">
+                    <a:fld id="{E58B2A00-6F64-4CE8-985E-600C21B8AFF3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -7282,7 +7275,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6B0B0E8-6CCA-4D7A-B8A0-AD08E04CD79B}" type="CELLRANGE">
+                    <a:fld id="{4E6DFCF6-C81C-45E4-9A69-C4F8E037A95D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -7504,11 +7497,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-917196800"/>
-        <c:axId val="-917199520"/>
+        <c:axId val="-1268795824"/>
+        <c:axId val="-1268794736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-917196800"/>
+        <c:axId val="-1268795824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7550,7 +7543,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-917199520"/>
+        <c:crossAx val="-1268794736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7558,7 +7551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-917199520"/>
+        <c:axId val="-1268794736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -7704,7 +7697,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-917196800"/>
+        <c:crossAx val="-1268795824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7925,7 +7918,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE3AE493-2886-44BE-9ED3-4A878FAC9003}" type="CELLRANGE">
+                    <a:fld id="{3115F517-4C44-48C7-B14E-1756A54CD12B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -7965,7 +7958,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1972561C-C906-4ED6-A570-F40B900E7798}" type="CELLRANGE">
+                    <a:fld id="{3E2972A3-B57B-4202-BC41-8C7A130E771C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -8005,7 +7998,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7ED453F4-6B3C-4848-B66F-997D05FBD7B5}" type="CELLRANGE">
+                    <a:fld id="{CBAB696F-1E7C-46A6-AF1C-1D7AF2C2505D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -8226,11 +8219,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-916658016"/>
-        <c:axId val="-916658560"/>
+        <c:axId val="-1268793648"/>
+        <c:axId val="-1268796912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-916658016"/>
+        <c:axId val="-1268793648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8269,7 +8262,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916658560"/>
+        <c:crossAx val="-1268796912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8277,7 +8270,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-916658560"/>
+        <c:axId val="-1268796912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -8421,7 +8414,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916658016"/>
+        <c:crossAx val="-1268793648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8931,11 +8924,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-916654752"/>
-        <c:axId val="-916659648"/>
+        <c:axId val="-1268791472"/>
+        <c:axId val="-1268786032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-916654752"/>
+        <c:axId val="-1268791472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8974,7 +8967,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916659648"/>
+        <c:crossAx val="-1268786032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8982,7 +8975,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-916659648"/>
+        <c:axId val="-1268786032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -9127,7 +9120,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916654752"/>
+        <c:crossAx val="-1268791472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9276,7 +9269,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{167AE597-A0AB-4848-A750-726BEDC7FF18}" type="CELLRANGE">
+                    <a:fld id="{90B3A3A9-68EC-437B-BE2A-96E5702AF016}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9311,7 +9304,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73A46B45-5B7F-40FB-880F-D5D090248651}" type="CELLRANGE">
+                    <a:fld id="{A891F364-3DD7-49FD-8E0B-D43C47B37CDD}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9344,7 +9337,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44326B63-A8E6-41A8-A7C4-FA3949000313}" type="CELLRANGE">
+                    <a:fld id="{AF7745C8-28EF-49B6-B44B-DC8AB895C785}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9475,11 +9468,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-916661824"/>
-        <c:axId val="-916664000"/>
+        <c:axId val="-1268798544"/>
+        <c:axId val="-1268789840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-916661824"/>
+        <c:axId val="-1268798544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9528,7 +9521,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916664000"/>
+        <c:crossAx val="-1268789840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9536,7 +9529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-916664000"/>
+        <c:axId val="-1268789840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9604,7 +9597,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916664000"/>
+        <c:crossAx val="-1268789840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9681,7 +9674,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC88AE32-E345-439F-B63A-14DEDE838E4E}" type="CELLRANGE">
+                    <a:fld id="{0A4F8CF6-8F1B-434B-9B90-CD0B0B64AD81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9716,7 +9709,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6DCA384-809A-4E9F-AA47-9837961251A6}" type="CELLRANGE">
+                    <a:fld id="{6F5D8AE4-8C68-4C44-92BA-4B39E8410DDA}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9749,7 +9742,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{555E173A-4990-4899-ACF0-5D9485CA4EDC}" type="CELLRANGE">
+                    <a:fld id="{8173917F-A583-44EC-A8A9-1F1857204E33}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9880,11 +9873,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-916650400"/>
-        <c:axId val="-916653120"/>
+        <c:axId val="-1268787664"/>
+        <c:axId val="-1268800176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-916650400"/>
+        <c:axId val="-1268787664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9954,7 +9947,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916653120"/>
+        <c:crossAx val="-1268800176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9962,7 +9955,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-916653120"/>
+        <c:axId val="-1268800176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10064,7 +10057,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916653120"/>
+        <c:crossAx val="-1268800176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10449,11 +10442,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-916654208"/>
-        <c:axId val="-916664544"/>
+        <c:axId val="-1268798000"/>
+        <c:axId val="-1268797456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-916654208"/>
+        <c:axId val="-1268798000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10476,7 +10469,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916664544"/>
+        <c:crossAx val="-1268797456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10484,7 +10477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-916664544"/>
+        <c:axId val="-1268797456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10551,7 +10544,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-916664544"/>
+        <c:crossAx val="-1268797456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13341,7 +13334,7 @@
         <xdr:cNvPr id="2" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13379,7 +13372,7 @@
         <xdr:cNvPr id="3" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13417,7 +13410,7 @@
         <xdr:cNvPr id="4" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13455,7 +13448,7 @@
         <xdr:cNvPr id="5" name="Graphique 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13493,7 +13486,7 @@
         <xdr:cNvPr id="6" name="Graphique 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13531,7 +13524,7 @@
         <xdr:cNvPr id="7" name="Graphique 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13569,7 +13562,7 @@
         <xdr:cNvPr id="8" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13607,7 +13600,7 @@
         <xdr:cNvPr id="9" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13645,7 +13638,7 @@
         <xdr:cNvPr id="10" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13683,7 +13676,7 @@
         <xdr:cNvPr id="11" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13721,7 +13714,7 @@
         <xdr:cNvPr id="12" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13759,7 +13752,7 @@
         <xdr:cNvPr id="13" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13797,7 +13790,7 @@
         <xdr:cNvPr id="14" name="Graphique 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13835,7 +13828,7 @@
         <xdr:cNvPr id="15" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13873,7 +13866,7 @@
         <xdr:cNvPr id="16" name="Graphique 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000025000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0E00-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13957,11 +13950,6 @@
             <v>1029000</v>
           </cell>
         </row>
-        <row r="17">
-          <cell r="E17">
-            <v>0</v>
-          </cell>
-        </row>
         <row r="21">
           <cell r="C21">
             <v>24</v>
@@ -13984,11 +13972,6 @@
             <v>1004560.78</v>
           </cell>
         </row>
-        <row r="27">
-          <cell r="E27">
-            <v>0</v>
-          </cell>
-        </row>
         <row r="31">
           <cell r="C31">
             <v>2</v>
@@ -14009,11 +13992,6 @@
           </cell>
           <cell r="E32">
             <v>230000</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="E40">
-            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -14182,51 +14160,19 @@
             <v>0</v>
           </cell>
         </row>
-        <row r="7">
-          <cell r="A7"/>
-          <cell r="B7"/>
-          <cell r="C7"/>
-          <cell r="E7"/>
-          <cell r="F7"/>
-          <cell r="G7"/>
-          <cell r="O7"/>
-          <cell r="R7"/>
-          <cell r="S7"/>
-          <cell r="T7"/>
-          <cell r="U7"/>
-          <cell r="V7"/>
-        </row>
-        <row r="8">
-          <cell r="A8"/>
-          <cell r="B8"/>
-          <cell r="C8"/>
-          <cell r="E8"/>
-          <cell r="F8"/>
-          <cell r="G8"/>
-          <cell r="O8"/>
-          <cell r="R8"/>
-          <cell r="S8"/>
-          <cell r="T8"/>
-          <cell r="U8"/>
-        </row>
         <row r="9">
           <cell r="A9">
             <v>165000</v>
           </cell>
-          <cell r="B9"/>
           <cell r="C9">
             <v>400000</v>
           </cell>
           <cell r="E9">
             <v>400000</v>
           </cell>
-          <cell r="F9"/>
           <cell r="G9">
             <v>0</v>
           </cell>
-          <cell r="O9"/>
-          <cell r="R9"/>
-          <cell r="S9"/>
           <cell r="T9">
             <v>0</v>
           </cell>
@@ -14236,604 +14182,6 @@
           <cell r="V9">
             <v>0</v>
           </cell>
-        </row>
-        <row r="10">
-          <cell r="A10"/>
-          <cell r="B10"/>
-          <cell r="C10"/>
-          <cell r="E10"/>
-          <cell r="F10"/>
-          <cell r="G10"/>
-          <cell r="O10"/>
-          <cell r="R10"/>
-          <cell r="S10"/>
-          <cell r="T10"/>
-          <cell r="U10"/>
-        </row>
-        <row r="11">
-          <cell r="A11"/>
-          <cell r="B11"/>
-          <cell r="C11"/>
-          <cell r="E11"/>
-          <cell r="F11"/>
-          <cell r="G11"/>
-          <cell r="O11"/>
-          <cell r="R11"/>
-          <cell r="S11"/>
-          <cell r="T11"/>
-          <cell r="U11"/>
-        </row>
-        <row r="12">
-          <cell r="A12"/>
-          <cell r="B12"/>
-          <cell r="C12"/>
-          <cell r="E12"/>
-          <cell r="F12"/>
-          <cell r="G12"/>
-          <cell r="O12"/>
-          <cell r="R12"/>
-          <cell r="S12"/>
-          <cell r="T12"/>
-          <cell r="U12"/>
-        </row>
-        <row r="13">
-          <cell r="A13"/>
-          <cell r="B13"/>
-          <cell r="C13"/>
-          <cell r="E13"/>
-          <cell r="F13"/>
-          <cell r="G13"/>
-          <cell r="O13"/>
-          <cell r="R13"/>
-          <cell r="S13"/>
-          <cell r="T13"/>
-          <cell r="U13"/>
-        </row>
-        <row r="14">
-          <cell r="A14"/>
-          <cell r="B14"/>
-          <cell r="C14"/>
-          <cell r="E14"/>
-          <cell r="F14"/>
-          <cell r="G14"/>
-          <cell r="O14"/>
-          <cell r="R14"/>
-          <cell r="S14"/>
-          <cell r="T14"/>
-          <cell r="U14"/>
-        </row>
-        <row r="15">
-          <cell r="A15"/>
-          <cell r="B15"/>
-          <cell r="C15"/>
-          <cell r="E15"/>
-          <cell r="F15"/>
-          <cell r="G15"/>
-          <cell r="O15"/>
-          <cell r="R15"/>
-          <cell r="S15"/>
-          <cell r="T15"/>
-          <cell r="U15"/>
-        </row>
-        <row r="16">
-          <cell r="A16"/>
-          <cell r="B16"/>
-          <cell r="C16"/>
-          <cell r="E16"/>
-          <cell r="F16"/>
-          <cell r="G16"/>
-          <cell r="O16"/>
-          <cell r="R16"/>
-          <cell r="S16"/>
-          <cell r="T16"/>
-          <cell r="U16"/>
-        </row>
-        <row r="17">
-          <cell r="A17"/>
-          <cell r="B17"/>
-          <cell r="C17"/>
-          <cell r="E17"/>
-          <cell r="F17"/>
-          <cell r="G17"/>
-          <cell r="O17"/>
-          <cell r="R17"/>
-          <cell r="S17"/>
-          <cell r="T17"/>
-          <cell r="U17"/>
-        </row>
-        <row r="18">
-          <cell r="A18"/>
-          <cell r="B18"/>
-          <cell r="C18"/>
-          <cell r="E18"/>
-          <cell r="F18"/>
-          <cell r="G18"/>
-          <cell r="O18"/>
-          <cell r="R18"/>
-          <cell r="S18"/>
-          <cell r="T18"/>
-          <cell r="U18"/>
-        </row>
-        <row r="19">
-          <cell r="A19"/>
-          <cell r="B19"/>
-          <cell r="C19"/>
-          <cell r="E19"/>
-          <cell r="F19"/>
-          <cell r="G19"/>
-          <cell r="O19"/>
-          <cell r="R19"/>
-          <cell r="S19"/>
-          <cell r="T19"/>
-          <cell r="U19"/>
-        </row>
-        <row r="20">
-          <cell r="A20"/>
-          <cell r="B20"/>
-          <cell r="C20"/>
-          <cell r="E20"/>
-          <cell r="F20"/>
-          <cell r="G20"/>
-          <cell r="O20"/>
-          <cell r="R20"/>
-          <cell r="S20"/>
-          <cell r="T20"/>
-          <cell r="U20"/>
-        </row>
-        <row r="21">
-          <cell r="A21"/>
-          <cell r="B21"/>
-          <cell r="C21"/>
-          <cell r="E21"/>
-          <cell r="F21"/>
-          <cell r="G21"/>
-          <cell r="O21"/>
-          <cell r="R21"/>
-          <cell r="S21"/>
-          <cell r="T21"/>
-          <cell r="U21"/>
-        </row>
-        <row r="22">
-          <cell r="A22"/>
-          <cell r="B22"/>
-          <cell r="C22"/>
-          <cell r="E22"/>
-          <cell r="F22"/>
-          <cell r="G22"/>
-          <cell r="O22"/>
-          <cell r="R22"/>
-          <cell r="S22"/>
-          <cell r="T22"/>
-          <cell r="U22"/>
-        </row>
-        <row r="23">
-          <cell r="A23"/>
-          <cell r="B23"/>
-          <cell r="C23"/>
-          <cell r="E23"/>
-          <cell r="F23"/>
-          <cell r="G23"/>
-          <cell r="O23"/>
-          <cell r="R23"/>
-          <cell r="S23"/>
-          <cell r="T23"/>
-          <cell r="U23"/>
-        </row>
-        <row r="24">
-          <cell r="A24"/>
-          <cell r="B24"/>
-          <cell r="C24"/>
-          <cell r="E24"/>
-          <cell r="F24"/>
-          <cell r="G24"/>
-          <cell r="O24"/>
-          <cell r="R24"/>
-          <cell r="S24"/>
-          <cell r="T24"/>
-          <cell r="U24"/>
-        </row>
-        <row r="25">
-          <cell r="A25"/>
-          <cell r="B25"/>
-          <cell r="C25"/>
-          <cell r="E25"/>
-          <cell r="F25"/>
-          <cell r="G25"/>
-          <cell r="O25"/>
-          <cell r="R25"/>
-          <cell r="S25"/>
-          <cell r="T25"/>
-          <cell r="U25"/>
-        </row>
-        <row r="26">
-          <cell r="A26"/>
-          <cell r="B26"/>
-          <cell r="C26"/>
-          <cell r="E26"/>
-          <cell r="F26"/>
-          <cell r="G26"/>
-          <cell r="O26"/>
-          <cell r="R26"/>
-          <cell r="S26"/>
-          <cell r="T26"/>
-          <cell r="U26"/>
-        </row>
-        <row r="27">
-          <cell r="A27"/>
-          <cell r="B27"/>
-          <cell r="C27"/>
-          <cell r="E27"/>
-          <cell r="F27"/>
-          <cell r="G27"/>
-          <cell r="O27"/>
-          <cell r="R27"/>
-          <cell r="S27"/>
-          <cell r="T27"/>
-          <cell r="U27"/>
-        </row>
-        <row r="28">
-          <cell r="A28"/>
-          <cell r="B28"/>
-          <cell r="C28"/>
-          <cell r="E28"/>
-          <cell r="F28"/>
-          <cell r="G28"/>
-          <cell r="O28"/>
-          <cell r="R28"/>
-          <cell r="S28"/>
-          <cell r="T28"/>
-          <cell r="U28"/>
-        </row>
-        <row r="29">
-          <cell r="A29"/>
-          <cell r="B29"/>
-          <cell r="C29"/>
-          <cell r="E29"/>
-          <cell r="F29"/>
-          <cell r="G29"/>
-          <cell r="O29"/>
-          <cell r="R29"/>
-          <cell r="S29"/>
-          <cell r="T29"/>
-          <cell r="U29"/>
-        </row>
-        <row r="30">
-          <cell r="A30"/>
-          <cell r="B30"/>
-          <cell r="C30"/>
-          <cell r="E30"/>
-          <cell r="F30"/>
-          <cell r="G30"/>
-          <cell r="O30"/>
-          <cell r="R30"/>
-          <cell r="S30"/>
-          <cell r="T30"/>
-          <cell r="U30"/>
-        </row>
-        <row r="31">
-          <cell r="A31"/>
-          <cell r="B31"/>
-          <cell r="C31"/>
-          <cell r="E31"/>
-          <cell r="F31"/>
-          <cell r="G31"/>
-          <cell r="O31"/>
-          <cell r="R31"/>
-          <cell r="S31"/>
-          <cell r="T31"/>
-          <cell r="U31"/>
-        </row>
-        <row r="32">
-          <cell r="A32"/>
-          <cell r="B32"/>
-          <cell r="C32"/>
-          <cell r="E32"/>
-          <cell r="F32"/>
-          <cell r="G32"/>
-          <cell r="O32"/>
-          <cell r="R32"/>
-          <cell r="S32"/>
-          <cell r="T32"/>
-          <cell r="U32"/>
-        </row>
-        <row r="33">
-          <cell r="A33"/>
-          <cell r="B33"/>
-          <cell r="C33"/>
-          <cell r="E33"/>
-          <cell r="F33"/>
-          <cell r="G33"/>
-          <cell r="O33"/>
-          <cell r="R33"/>
-          <cell r="S33"/>
-          <cell r="T33"/>
-          <cell r="U33"/>
-        </row>
-        <row r="34">
-          <cell r="A34"/>
-          <cell r="B34"/>
-          <cell r="C34"/>
-          <cell r="E34"/>
-          <cell r="F34"/>
-          <cell r="G34"/>
-          <cell r="O34"/>
-          <cell r="R34"/>
-          <cell r="S34"/>
-          <cell r="T34"/>
-          <cell r="U34"/>
-        </row>
-        <row r="35">
-          <cell r="A35"/>
-          <cell r="B35"/>
-          <cell r="C35"/>
-          <cell r="E35"/>
-          <cell r="F35"/>
-          <cell r="G35"/>
-          <cell r="O35"/>
-          <cell r="R35"/>
-          <cell r="S35"/>
-          <cell r="T35"/>
-          <cell r="U35"/>
-        </row>
-        <row r="36">
-          <cell r="A36"/>
-          <cell r="B36"/>
-          <cell r="C36"/>
-          <cell r="E36"/>
-          <cell r="F36"/>
-          <cell r="G36"/>
-          <cell r="O36"/>
-          <cell r="R36"/>
-          <cell r="S36"/>
-          <cell r="T36"/>
-          <cell r="U36"/>
-        </row>
-        <row r="37">
-          <cell r="A37"/>
-          <cell r="B37"/>
-          <cell r="C37"/>
-          <cell r="E37"/>
-          <cell r="F37"/>
-          <cell r="G37"/>
-          <cell r="O37"/>
-          <cell r="R37"/>
-          <cell r="S37"/>
-          <cell r="T37"/>
-          <cell r="U37"/>
-        </row>
-        <row r="38">
-          <cell r="A38"/>
-          <cell r="B38"/>
-          <cell r="C38"/>
-          <cell r="E38"/>
-          <cell r="F38"/>
-          <cell r="G38"/>
-          <cell r="O38"/>
-          <cell r="R38"/>
-          <cell r="S38"/>
-          <cell r="T38"/>
-          <cell r="U38"/>
-        </row>
-        <row r="39">
-          <cell r="A39"/>
-          <cell r="B39"/>
-          <cell r="C39"/>
-          <cell r="E39"/>
-          <cell r="F39"/>
-          <cell r="G39"/>
-          <cell r="O39"/>
-          <cell r="R39"/>
-          <cell r="S39"/>
-          <cell r="T39"/>
-          <cell r="U39"/>
-        </row>
-        <row r="40">
-          <cell r="A40"/>
-          <cell r="B40"/>
-          <cell r="C40"/>
-          <cell r="E40"/>
-          <cell r="F40"/>
-          <cell r="G40"/>
-          <cell r="O40"/>
-          <cell r="R40"/>
-          <cell r="S40"/>
-          <cell r="T40"/>
-          <cell r="U40"/>
-        </row>
-        <row r="41">
-          <cell r="A41"/>
-          <cell r="B41"/>
-          <cell r="C41"/>
-          <cell r="E41"/>
-          <cell r="F41"/>
-          <cell r="G41"/>
-          <cell r="O41"/>
-          <cell r="R41"/>
-          <cell r="S41"/>
-          <cell r="T41"/>
-          <cell r="U41"/>
-        </row>
-        <row r="42">
-          <cell r="A42"/>
-          <cell r="B42"/>
-          <cell r="C42"/>
-          <cell r="E42"/>
-          <cell r="F42"/>
-          <cell r="G42"/>
-          <cell r="O42"/>
-          <cell r="R42"/>
-          <cell r="S42"/>
-          <cell r="T42"/>
-          <cell r="U42"/>
-        </row>
-        <row r="43">
-          <cell r="A43"/>
-          <cell r="B43"/>
-          <cell r="C43"/>
-          <cell r="E43"/>
-          <cell r="F43"/>
-          <cell r="G43"/>
-          <cell r="O43"/>
-          <cell r="R43"/>
-          <cell r="S43"/>
-          <cell r="T43"/>
-          <cell r="U43"/>
-        </row>
-        <row r="44">
-          <cell r="A44"/>
-          <cell r="B44"/>
-          <cell r="C44"/>
-          <cell r="E44"/>
-          <cell r="F44"/>
-          <cell r="G44"/>
-          <cell r="O44"/>
-          <cell r="R44"/>
-          <cell r="S44"/>
-          <cell r="T44"/>
-          <cell r="U44"/>
-        </row>
-        <row r="45">
-          <cell r="A45"/>
-          <cell r="B45"/>
-          <cell r="C45"/>
-          <cell r="E45"/>
-          <cell r="F45"/>
-          <cell r="G45"/>
-          <cell r="O45"/>
-          <cell r="R45"/>
-          <cell r="S45"/>
-          <cell r="T45"/>
-          <cell r="U45"/>
-        </row>
-        <row r="46">
-          <cell r="A46"/>
-          <cell r="B46"/>
-          <cell r="C46"/>
-          <cell r="E46"/>
-          <cell r="F46"/>
-          <cell r="G46"/>
-          <cell r="O46"/>
-          <cell r="R46"/>
-          <cell r="S46"/>
-          <cell r="T46"/>
-          <cell r="U46"/>
-        </row>
-        <row r="47">
-          <cell r="A47"/>
-          <cell r="B47"/>
-          <cell r="C47"/>
-          <cell r="E47"/>
-          <cell r="F47"/>
-          <cell r="G47"/>
-          <cell r="O47"/>
-          <cell r="R47"/>
-          <cell r="S47"/>
-          <cell r="T47"/>
-          <cell r="U47"/>
-        </row>
-        <row r="48">
-          <cell r="A48"/>
-          <cell r="B48"/>
-          <cell r="C48"/>
-          <cell r="E48"/>
-          <cell r="F48"/>
-          <cell r="G48"/>
-          <cell r="O48"/>
-          <cell r="R48"/>
-          <cell r="S48"/>
-          <cell r="T48"/>
-          <cell r="U48"/>
-        </row>
-        <row r="49">
-          <cell r="A49"/>
-          <cell r="B49"/>
-          <cell r="C49"/>
-          <cell r="E49"/>
-          <cell r="F49"/>
-          <cell r="G49"/>
-          <cell r="O49"/>
-          <cell r="R49"/>
-          <cell r="S49"/>
-          <cell r="T49"/>
-          <cell r="U49"/>
-        </row>
-        <row r="50">
-          <cell r="A50"/>
-          <cell r="B50"/>
-          <cell r="C50"/>
-          <cell r="E50"/>
-          <cell r="F50"/>
-          <cell r="G50"/>
-          <cell r="O50"/>
-          <cell r="R50"/>
-          <cell r="S50"/>
-          <cell r="T50"/>
-          <cell r="U50"/>
-        </row>
-        <row r="51">
-          <cell r="A51"/>
-          <cell r="B51"/>
-          <cell r="C51"/>
-          <cell r="E51"/>
-          <cell r="F51"/>
-          <cell r="G51"/>
-          <cell r="O51"/>
-          <cell r="R51"/>
-          <cell r="S51"/>
-          <cell r="T51"/>
-          <cell r="U51"/>
-        </row>
-        <row r="52">
-          <cell r="A52"/>
-          <cell r="B52"/>
-          <cell r="C52"/>
-          <cell r="E52"/>
-          <cell r="F52"/>
-          <cell r="G52"/>
-          <cell r="O52"/>
-          <cell r="R52"/>
-          <cell r="S52"/>
-          <cell r="T52"/>
-          <cell r="U52"/>
-        </row>
-        <row r="53">
-          <cell r="A53"/>
-          <cell r="B53"/>
-          <cell r="C53"/>
-          <cell r="E53"/>
-          <cell r="F53"/>
-          <cell r="G53"/>
-          <cell r="O53"/>
-          <cell r="R53"/>
-          <cell r="S53"/>
-          <cell r="T53"/>
-          <cell r="U53"/>
-        </row>
-        <row r="54">
-          <cell r="A54"/>
-          <cell r="B54"/>
-          <cell r="C54"/>
-          <cell r="E54"/>
-          <cell r="F54"/>
-          <cell r="G54"/>
-          <cell r="O54"/>
-          <cell r="R54"/>
-          <cell r="S54"/>
-          <cell r="T54"/>
-          <cell r="U54"/>
-        </row>
-        <row r="55">
-          <cell r="A55"/>
-          <cell r="B55"/>
-          <cell r="C55"/>
-          <cell r="E55"/>
-          <cell r="F55"/>
-          <cell r="G55"/>
-          <cell r="O55"/>
-          <cell r="R55"/>
-          <cell r="S55"/>
-          <cell r="T55"/>
-          <cell r="U55"/>
         </row>
       </sheetData>
       <sheetData sheetId="10">
@@ -14887,264 +14235,6 @@
             <v>0</v>
           </cell>
         </row>
-        <row r="6">
-          <cell r="A6"/>
-          <cell r="C6"/>
-          <cell r="D6"/>
-          <cell r="F6"/>
-          <cell r="H6"/>
-          <cell r="L6"/>
-          <cell r="O6"/>
-          <cell r="P6"/>
-          <cell r="T6"/>
-          <cell r="W6"/>
-          <cell r="X6"/>
-          <cell r="AB6"/>
-          <cell r="AE6"/>
-          <cell r="AF6"/>
-          <cell r="AG6"/>
-          <cell r="AH6"/>
-        </row>
-        <row r="7">
-          <cell r="A7"/>
-          <cell r="C7"/>
-          <cell r="D7"/>
-          <cell r="F7"/>
-          <cell r="H7"/>
-          <cell r="L7"/>
-          <cell r="O7"/>
-          <cell r="P7"/>
-          <cell r="T7"/>
-          <cell r="W7"/>
-          <cell r="X7"/>
-          <cell r="AB7"/>
-          <cell r="AE7"/>
-        </row>
-        <row r="8">
-          <cell r="A8"/>
-          <cell r="C8"/>
-          <cell r="D8"/>
-          <cell r="F8"/>
-          <cell r="H8"/>
-          <cell r="L8"/>
-          <cell r="O8"/>
-          <cell r="P8"/>
-          <cell r="T8"/>
-          <cell r="W8"/>
-          <cell r="X8"/>
-          <cell r="AB8"/>
-          <cell r="AE8"/>
-        </row>
-        <row r="9">
-          <cell r="A9"/>
-          <cell r="C9"/>
-          <cell r="D9"/>
-          <cell r="F9"/>
-          <cell r="H9"/>
-          <cell r="L9"/>
-          <cell r="O9"/>
-          <cell r="P9"/>
-          <cell r="T9"/>
-          <cell r="W9"/>
-          <cell r="X9"/>
-          <cell r="AB9"/>
-          <cell r="AE9"/>
-        </row>
-        <row r="10">
-          <cell r="A10"/>
-          <cell r="C10"/>
-          <cell r="D10"/>
-          <cell r="F10"/>
-          <cell r="H10"/>
-          <cell r="L10"/>
-          <cell r="O10"/>
-          <cell r="P10"/>
-          <cell r="T10"/>
-          <cell r="W10"/>
-          <cell r="X10"/>
-          <cell r="AB10"/>
-          <cell r="AE10"/>
-        </row>
-        <row r="11">
-          <cell r="A11"/>
-          <cell r="C11"/>
-          <cell r="D11"/>
-          <cell r="F11"/>
-          <cell r="H11"/>
-          <cell r="L11"/>
-          <cell r="O11"/>
-          <cell r="P11"/>
-          <cell r="T11"/>
-          <cell r="W11"/>
-          <cell r="X11"/>
-          <cell r="AB11"/>
-          <cell r="AE11"/>
-        </row>
-        <row r="12">
-          <cell r="A12"/>
-          <cell r="C12"/>
-          <cell r="D12"/>
-          <cell r="F12"/>
-          <cell r="H12"/>
-          <cell r="L12"/>
-          <cell r="O12"/>
-          <cell r="P12"/>
-          <cell r="T12"/>
-          <cell r="W12"/>
-          <cell r="X12"/>
-          <cell r="AB12"/>
-          <cell r="AE12"/>
-        </row>
-        <row r="13">
-          <cell r="A13"/>
-          <cell r="C13"/>
-          <cell r="D13"/>
-          <cell r="F13"/>
-          <cell r="H13"/>
-          <cell r="L13"/>
-          <cell r="O13"/>
-          <cell r="P13"/>
-          <cell r="T13"/>
-          <cell r="W13"/>
-          <cell r="X13"/>
-          <cell r="AB13"/>
-          <cell r="AE13"/>
-        </row>
-        <row r="14">
-          <cell r="A14"/>
-          <cell r="C14"/>
-          <cell r="D14"/>
-          <cell r="F14"/>
-          <cell r="H14"/>
-          <cell r="L14"/>
-          <cell r="O14"/>
-          <cell r="P14"/>
-          <cell r="T14"/>
-          <cell r="W14"/>
-          <cell r="X14"/>
-          <cell r="AB14"/>
-          <cell r="AE14"/>
-        </row>
-        <row r="15">
-          <cell r="A15"/>
-          <cell r="C15"/>
-          <cell r="D15"/>
-          <cell r="F15"/>
-          <cell r="H15"/>
-          <cell r="L15"/>
-          <cell r="O15"/>
-          <cell r="P15"/>
-          <cell r="T15"/>
-          <cell r="W15"/>
-          <cell r="X15"/>
-          <cell r="AB15"/>
-          <cell r="AE15"/>
-        </row>
-        <row r="16">
-          <cell r="A16"/>
-          <cell r="C16"/>
-          <cell r="D16"/>
-          <cell r="F16"/>
-          <cell r="H16"/>
-          <cell r="L16"/>
-          <cell r="O16"/>
-          <cell r="P16"/>
-          <cell r="T16"/>
-          <cell r="W16"/>
-          <cell r="X16"/>
-          <cell r="AB16"/>
-          <cell r="AE16"/>
-        </row>
-        <row r="17">
-          <cell r="A17"/>
-          <cell r="C17"/>
-          <cell r="D17"/>
-          <cell r="F17"/>
-          <cell r="H17"/>
-          <cell r="L17"/>
-          <cell r="O17"/>
-          <cell r="P17"/>
-          <cell r="T17"/>
-          <cell r="W17"/>
-          <cell r="X17"/>
-          <cell r="AB17"/>
-          <cell r="AE17"/>
-        </row>
-        <row r="18">
-          <cell r="A18"/>
-          <cell r="C18"/>
-          <cell r="D18"/>
-          <cell r="F18"/>
-          <cell r="H18"/>
-          <cell r="L18"/>
-          <cell r="O18"/>
-          <cell r="P18"/>
-          <cell r="T18"/>
-          <cell r="W18"/>
-          <cell r="X18"/>
-          <cell r="AB18"/>
-          <cell r="AE18"/>
-        </row>
-        <row r="19">
-          <cell r="A19"/>
-          <cell r="C19"/>
-          <cell r="D19"/>
-          <cell r="F19"/>
-          <cell r="H19"/>
-          <cell r="L19"/>
-          <cell r="O19"/>
-          <cell r="P19"/>
-          <cell r="T19"/>
-          <cell r="W19"/>
-          <cell r="X19"/>
-          <cell r="AB19"/>
-          <cell r="AE19"/>
-        </row>
-        <row r="20">
-          <cell r="A20"/>
-          <cell r="C20"/>
-          <cell r="D20"/>
-          <cell r="F20"/>
-          <cell r="H20"/>
-          <cell r="L20"/>
-          <cell r="O20"/>
-          <cell r="P20"/>
-          <cell r="T20"/>
-          <cell r="W20"/>
-          <cell r="X20"/>
-          <cell r="AB20"/>
-          <cell r="AE20"/>
-        </row>
-        <row r="21">
-          <cell r="A21"/>
-          <cell r="C21"/>
-          <cell r="D21"/>
-          <cell r="F21"/>
-          <cell r="H21"/>
-          <cell r="L21"/>
-          <cell r="O21"/>
-          <cell r="P21"/>
-          <cell r="T21"/>
-          <cell r="W21"/>
-          <cell r="X21"/>
-          <cell r="AB21"/>
-          <cell r="AE21"/>
-        </row>
-        <row r="22">
-          <cell r="A22"/>
-          <cell r="C22"/>
-          <cell r="D22"/>
-          <cell r="F22"/>
-          <cell r="H22"/>
-          <cell r="L22"/>
-          <cell r="O22"/>
-          <cell r="P22"/>
-          <cell r="T22"/>
-          <cell r="W22"/>
-          <cell r="X22"/>
-          <cell r="AB22"/>
-          <cell r="AE22"/>
-        </row>
       </sheetData>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12">
@@ -15168,7 +14258,6 @@
           </cell>
         </row>
         <row r="5">
-          <cell r="K5"/>
           <cell r="L5"/>
           <cell r="P5">
             <v>202300</v>
@@ -15178,7 +14267,6 @@
           </cell>
         </row>
         <row r="6">
-          <cell r="K6"/>
           <cell r="L6"/>
           <cell r="P6">
             <v>426700</v>
@@ -15188,7 +14276,6 @@
           </cell>
         </row>
         <row r="7">
-          <cell r="K7"/>
           <cell r="L7"/>
           <cell r="P7">
             <v>400000</v>
@@ -15207,14 +14294,7 @@
             <v>780000</v>
           </cell>
         </row>
-        <row r="10">
-          <cell r="K10"/>
-        </row>
-        <row r="11">
-          <cell r="K11"/>
-        </row>
         <row r="12">
-          <cell r="K12"/>
           <cell r="P12">
             <v>46</v>
           </cell>
@@ -15243,15 +14323,6 @@
           <cell r="R14">
             <v>3.5087719298245612E-2</v>
           </cell>
-        </row>
-        <row r="15">
-          <cell r="K15"/>
-        </row>
-        <row r="16">
-          <cell r="K16"/>
-        </row>
-        <row r="17">
-          <cell r="K17"/>
         </row>
         <row r="25">
           <cell r="B25">
@@ -15312,8 +14383,6 @@
           <cell r="B30">
             <v>0</v>
           </cell>
-          <cell r="D30"/>
-          <cell r="F30"/>
         </row>
         <row r="54">
           <cell r="B54">
@@ -15322,7 +14391,9 @@
           <cell r="C54">
             <v>168200</v>
           </cell>
-          <cell r="D54"/>
+          <cell r="E54">
+            <v>0</v>
+          </cell>
         </row>
         <row r="55">
           <cell r="B55">
@@ -15331,6 +14402,7 @@
           <cell r="C55">
             <v>249000</v>
           </cell>
+          <cell r="E55"/>
         </row>
         <row r="56">
           <cell r="B56">
@@ -15339,6 +14411,7 @@
           <cell r="C56">
             <v>348500</v>
           </cell>
+          <cell r="E56"/>
         </row>
         <row r="57">
           <cell r="B57">
@@ -15350,6 +14423,9 @@
           <cell r="D57">
             <v>0</v>
           </cell>
+          <cell r="E57">
+            <v>0</v>
+          </cell>
         </row>
         <row r="58">
           <cell r="B58">
@@ -15358,6 +14434,7 @@
           <cell r="C58">
             <v>240733</v>
           </cell>
+          <cell r="E58"/>
         </row>
         <row r="59">
           <cell r="B59">
@@ -15366,6 +14443,7 @@
           <cell r="C59">
             <v>167568</v>
           </cell>
+          <cell r="E59"/>
         </row>
         <row r="60">
           <cell r="B60">
@@ -15375,6 +14453,9 @@
           <cell r="D60">
             <v>620500</v>
           </cell>
+          <cell r="E60">
+            <v>0</v>
+          </cell>
         </row>
         <row r="61">
           <cell r="B61">
@@ -15383,6 +14464,7 @@
           <cell r="C61">
             <v>63700</v>
           </cell>
+          <cell r="E61"/>
         </row>
         <row r="62">
           <cell r="B62">
@@ -15391,6 +14473,7 @@
           <cell r="C62">
             <v>65000</v>
           </cell>
+          <cell r="E62"/>
         </row>
         <row r="73">
           <cell r="A73" t="str">
@@ -15795,8 +14878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N158" sqref="C157:N200"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15857,19 +14940,19 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="74" t="s">
         <v>106</v>
       </c>
       <c r="F4" s="41" t="s">
@@ -15880,22 +14963,22 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="106" t="s">
+      <c r="A5" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="126">
+      <c r="B5" s="124">
         <f>[1]Graphs!$P5/1000000</f>
         <v>0.20230000000000001</v>
       </c>
-      <c r="C5" s="109">
+      <c r="C5" s="107">
         <f>[1]Graphs!$R5</f>
         <v>0.19659863945578232</v>
       </c>
-      <c r="D5" s="127">
+      <c r="D5" s="125">
         <f>[1]Graphs!$P12</f>
         <v>46</v>
       </c>
-      <c r="E5" s="128">
+      <c r="E5" s="126">
         <f>[1]Graphs!$R12</f>
         <v>0.80701754385964908</v>
       </c>
@@ -15909,22 +14992,22 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="126">
+      <c r="B6" s="124">
         <f>[1]Graphs!$P6/1000000</f>
         <v>0.42670000000000002</v>
       </c>
-      <c r="C6" s="109">
+      <c r="C6" s="107">
         <f>[1]Graphs!$R6</f>
         <v>0.41467444120505342</v>
       </c>
-      <c r="D6" s="127">
+      <c r="D6" s="125">
         <f>[1]Graphs!$P13</f>
         <v>9</v>
       </c>
-      <c r="E6" s="128">
+      <c r="E6" s="126">
         <f>[1]Graphs!$R13</f>
         <v>0.15789473684210525</v>
       </c>
@@ -15938,22 +15021,22 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="126">
+      <c r="B7" s="124">
         <f>[1]Graphs!$P7/1000000</f>
         <v>0.4</v>
       </c>
-      <c r="C7" s="109">
+      <c r="C7" s="107">
         <f>[1]Graphs!$R7</f>
         <v>0.38872691933916426</v>
       </c>
-      <c r="D7" s="127">
+      <c r="D7" s="125">
         <f>[1]Graphs!$P14</f>
         <v>2</v>
       </c>
-      <c r="E7" s="128">
+      <c r="E7" s="126">
         <f>[1]Graphs!$R14</f>
         <v>3.5087719298245612E-2</v>
       </c>
@@ -15967,22 +15050,22 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="104" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="126">
+      <c r="B8" s="124">
         <f>SUM(B5:B7)</f>
         <v>1.0289999999999999</v>
       </c>
-      <c r="C8" s="109">
+      <c r="C8" s="107">
         <f>SUM(C5:C7)</f>
         <v>1</v>
       </c>
-      <c r="D8" s="110">
+      <c r="D8" s="108">
         <f>SUM(D5:D7)</f>
         <v>57</v>
       </c>
-      <c r="E8" s="109">
+      <c r="E8" s="107">
         <f>SUM(E5:E7)</f>
         <v>0.99999999999999989</v>
       </c>
@@ -16008,20 +15091,20 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="76" t="str">
+      <c r="A12" s="74" t="str">
         <f>A1</f>
         <v>Cyprus in 2018</v>
       </c>
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="107" t="s">
+      <c r="D12" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="107" t="s">
+      <c r="E12" s="105" t="s">
         <v>99</v>
       </c>
       <c r="F12" s="41" t="s">
@@ -16032,89 +15115,89 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="105">
+      <c r="B13" s="103">
         <f>[1]Graphs!$L$3</f>
         <v>30</v>
       </c>
-      <c r="C13" s="105">
+      <c r="C13" s="103">
         <f>[1]Graphs!$K$3</f>
         <v>168200</v>
       </c>
-      <c r="D13" s="104">
+      <c r="D13" s="102">
         <f>C13/SUM($C$13:$C$14)</f>
         <v>0.16345966958211855</v>
       </c>
-      <c r="E13" s="104">
+      <c r="E13" s="102">
         <f>B13/SUM($B$13:$B$14)</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="F13" s="101">
+      <c r="F13" s="99">
         <f>IF(D13&lt;0.0005,"",D13)</f>
         <v>0.16345966958211855</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="99">
         <f>IF(E13&lt;0.0005,"",E13)</f>
         <v>0.52631578947368418</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="106" t="s">
+      <c r="A14" s="104" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="105">
+      <c r="B14" s="103">
         <f>[1]Graphs!$L$4</f>
         <v>27</v>
       </c>
-      <c r="C14" s="105">
+      <c r="C14" s="103">
         <f>[1]Graphs!$K$4</f>
         <v>860800</v>
       </c>
-      <c r="D14" s="104">
+      <c r="D14" s="102">
         <f>C14/SUM($C$13:$C$14)</f>
         <v>0.83654033041788145</v>
       </c>
-      <c r="E14" s="104">
+      <c r="E14" s="102">
         <f>B14/SUM($B$13:$B$14)</f>
         <v>0.47368421052631576</v>
       </c>
-      <c r="F14" s="101">
+      <c r="F14" s="99">
         <f>IF(D14&lt;0.0005,"",D14)</f>
         <v>0.83654033041788145</v>
       </c>
-      <c r="G14" s="101">
+      <c r="G14" s="99">
         <f>IF(E14&lt;0.0005,"",E14)</f>
         <v>0.47368421052631576</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="98" t="s">
+      <c r="A15" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="98">
+      <c r="B15" s="96">
         <f>SUM(B14:B14)</f>
         <v>27</v>
       </c>
-      <c r="C15" s="103">
+      <c r="C15" s="101">
         <f>SUM(C14:C14)</f>
         <v>860800</v>
       </c>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="93" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="129">
-        <f>[1]Graphs!$L$6+[1]Graphs!$L$7++[1]Graphs!$L$5</f>
+      <c r="B16" s="127">
+        <f>[1]Graphs!$L$6+[1]Graphs!$L$7+[1]Graphs!$L$5</f>
         <v>0</v>
       </c>
-      <c r="C16" s="129">
+      <c r="C16" s="127">
         <f>+[1]Graphs!$K$6+[1]Graphs!$K$7+[1]Graphs!$K$5</f>
         <v>0</v>
       </c>
@@ -16129,28 +15212,28 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="76" t="s">
+      <c r="D20" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="76" t="s">
+      <c r="E20" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="76" t="s">
+      <c r="F20" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="76" t="s">
+      <c r="G20" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="76" t="s">
+      <c r="H20" s="74" t="s">
         <v>72</v>
       </c>
       <c r="I20" s="41" t="s">
@@ -16158,35 +15241,35 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="100">
+      <c r="A21" s="98">
         <f>[1]Graphs!$K$14</f>
         <v>646500</v>
       </c>
-      <c r="B21" s="100">
+      <c r="B21" s="98">
         <f>[1]Graphs!$K$15+[1]Graphs!$K$16+[1]Graphs!$K$17</f>
         <v>0</v>
       </c>
-      <c r="C21" s="99">
+      <c r="C21" s="97">
         <f>[1]Graphs!$K$13</f>
         <v>348500</v>
       </c>
-      <c r="D21" s="98">
+      <c r="D21" s="96">
         <f>D23-4</f>
         <v>2014</v>
       </c>
-      <c r="E21" s="97">
+      <c r="E21" s="95">
         <f>(A21+B21)/1000000</f>
         <v>0.64649999999999996</v>
       </c>
-      <c r="F21" s="97">
+      <c r="F21" s="95">
         <f>C21/1000000</f>
         <v>0.34849999999999998</v>
       </c>
-      <c r="G21" s="97">
+      <c r="G21" s="95">
         <f>SUM(E21:F21)</f>
         <v>0.99499999999999988</v>
       </c>
-      <c r="H21" s="96">
+      <c r="H21" s="94">
         <f>E21/G21</f>
         <v>0.64974874371859304</v>
       </c>
@@ -16196,35 +15279,35 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="100">
+      <c r="A22" s="98">
         <f>[1]Graphs!$K$9</f>
         <v>780000</v>
       </c>
-      <c r="B22" s="100">
+      <c r="B22" s="98">
         <f>[1]Graphs!$K$10+[1]Graphs!$K$11+[1]Graphs!$K$12</f>
         <v>0</v>
       </c>
-      <c r="C22" s="99">
+      <c r="C22" s="97">
         <f>[1]Graphs!$K$8</f>
         <v>249000</v>
       </c>
-      <c r="D22" s="98">
+      <c r="D22" s="96">
         <f>D23-2</f>
         <v>2016</v>
       </c>
-      <c r="E22" s="97">
+      <c r="E22" s="95">
         <f>(A22+B22)/1000000</f>
         <v>0.78</v>
       </c>
-      <c r="F22" s="97">
+      <c r="F22" s="95">
         <f>C22/1000000</f>
         <v>0.249</v>
       </c>
-      <c r="G22" s="97">
+      <c r="G22" s="95">
         <f>SUM(E22:F22)</f>
         <v>1.0289999999999999</v>
       </c>
-      <c r="H22" s="96">
+      <c r="H22" s="94">
         <f>E22/G22</f>
         <v>0.75801749271137031</v>
       </c>
@@ -16234,35 +15317,35 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="100">
+      <c r="A23" s="98">
         <f>[1]Graphs!$K$4</f>
         <v>860800</v>
       </c>
-      <c r="B23" s="100">
+      <c r="B23" s="98">
         <f>[1]Graphs!$K$5+[1]Graphs!$K$6+[1]Graphs!$K$7</f>
         <v>0</v>
       </c>
-      <c r="C23" s="99">
+      <c r="C23" s="97">
         <f>[1]Graphs!$K$3</f>
         <v>168200</v>
       </c>
-      <c r="D23" s="111" t="str">
+      <c r="D23" s="109" t="str">
         <f>[1]Graphs!$B$3</f>
         <v xml:space="preserve">2018 </v>
       </c>
-      <c r="E23" s="97">
+      <c r="E23" s="95">
         <f>(A23+B23)/1000000</f>
         <v>0.86080000000000001</v>
       </c>
-      <c r="F23" s="97">
+      <c r="F23" s="95">
         <f>C23/1000000</f>
         <v>0.16819999999999999</v>
       </c>
-      <c r="G23" s="97">
+      <c r="G23" s="95">
         <f>SUM(E23:F23)</f>
         <v>1.0289999999999999</v>
       </c>
-      <c r="H23" s="96">
+      <c r="H23" s="94">
         <f>E23/G23</f>
         <v>0.83654033041788156</v>
       </c>
@@ -16288,81 +15371,81 @@
     </row>
     <row r="39" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="162" t="str">
+      <c r="A40" s="152" t="str">
         <f>A1</f>
         <v>Cyprus in 2018</v>
       </c>
-      <c r="B40" s="174" t="s">
+      <c r="B40" s="155" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="160"/>
-      <c r="D40" s="161"/>
+      <c r="C40" s="156"/>
+      <c r="D40" s="157"/>
       <c r="E40" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="F40" s="160"/>
-      <c r="G40" s="161"/>
+      <c r="F40" s="156"/>
+      <c r="G40" s="157"/>
     </row>
     <row r="41" spans="1:21" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="163"/>
-      <c r="B41" s="80" t="s">
+      <c r="A41" s="153"/>
+      <c r="B41" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="80" t="s">
+      <c r="C41" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="79" t="s">
+      <c r="D41" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="E41" s="81" t="s">
+      <c r="E41" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="F41" s="80" t="s">
+      <c r="F41" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="G41" s="79" t="s">
+      <c r="G41" s="77" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="173"/>
-      <c r="B42" s="80" t="s">
+      <c r="A42" s="154"/>
+      <c r="B42" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="94" t="s">
+      <c r="C42" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="93" t="s">
+      <c r="D42" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="E42" s="94" t="s">
+      <c r="E42" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="94" t="s">
+      <c r="F42" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="93" t="s">
+      <c r="G42" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="J42" s="76" t="s">
+      <c r="J42" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="K42" s="76" t="s">
+      <c r="K42" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="L42" s="76" t="s">
+      <c r="L42" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="M42" s="76" t="s">
+      <c r="M42" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="N42" s="76" t="s">
+      <c r="N42" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="O42" s="76" t="s">
+      <c r="O42" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="P42" s="76" t="s">
+      <c r="P42" s="74" t="s">
         <v>84</v>
       </c>
       <c r="Q42" s="41" t="s">
@@ -16370,49 +15453,49 @@
       </c>
     </row>
     <row r="43" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="71" t="s">
+      <c r="A43" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="92">
+      <c r="B43" s="90">
         <f>[1]Summary_legal_compliance!$C$16</f>
         <v>57</v>
       </c>
-      <c r="C43" s="90">
+      <c r="C43" s="88">
         <f>[1]Summary_legal_compliance!$C$15</f>
         <v>27</v>
       </c>
-      <c r="D43" s="89">
+      <c r="D43" s="87">
         <f>[1]Summary_legal_compliance!$D$15</f>
         <v>47.368421052632002</v>
       </c>
-      <c r="E43" s="88">
+      <c r="E43" s="86">
         <f>[1]Summary_legal_compliance!$E$16</f>
         <v>1029000</v>
       </c>
-      <c r="F43" s="88">
+      <c r="F43" s="86">
         <f>[1]Summary_legal_compliance!$E$15</f>
         <v>860800</v>
       </c>
-      <c r="G43" s="87">
+      <c r="G43" s="85">
         <f>[1]Summary_legal_compliance!$F$15</f>
         <v>83.654033041787997</v>
       </c>
-      <c r="I43" s="71" t="s">
+      <c r="I43" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="J43" s="61">
+      <c r="J43" s="59">
         <f>[1]Graphs!$B$54/1000000</f>
         <v>0.86080000000000001</v>
       </c>
-      <c r="K43" s="61">
+      <c r="K43" s="59">
         <f>[1]Graphs!$C$54/1000000</f>
         <v>0.16819999999999999</v>
       </c>
-      <c r="L43" s="61">
+      <c r="L43" s="59">
         <f>E85</f>
         <v>0</v>
       </c>
-      <c r="M43" s="61">
+      <c r="M43" s="59">
         <f>$B$8</f>
         <v>1.0289999999999999</v>
       </c>
@@ -16424,7 +15507,7 @@
         <f>K43/(J43+K43)</f>
         <v>0.16345966958211858</v>
       </c>
-      <c r="P43" s="59">
+      <c r="P43" s="57">
         <f>[1]Graphs!$D$54/([1]Graphs!$D$54+[1]Graphs!$B$54+[1]Graphs!$C$54)</f>
         <v>0</v>
       </c>
@@ -16434,49 +15517,49 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="71" t="s">
+      <c r="A44" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="91">
+      <c r="B44" s="89">
         <f>[1]Summary_legal_compliance!$C$22</f>
         <v>54</v>
       </c>
-      <c r="C44" s="90">
+      <c r="C44" s="88">
         <f>[1]Summary_legal_compliance!$C$21</f>
         <v>24</v>
       </c>
-      <c r="D44" s="89">
+      <c r="D44" s="87">
         <f>[1]Summary_legal_compliance!$D$21</f>
         <v>44.444444444444002</v>
       </c>
-      <c r="E44" s="88">
+      <c r="E44" s="86">
         <f>[1]Summary_legal_compliance!$E$22</f>
         <v>1004560.78</v>
       </c>
-      <c r="F44" s="88">
+      <c r="F44" s="86">
         <f>[1]Summary_legal_compliance!$E$21</f>
         <v>844150.08</v>
       </c>
-      <c r="G44" s="87">
+      <c r="G44" s="85">
         <f>[1]Summary_legal_compliance!$F$21</f>
         <v>84.031757640389003</v>
       </c>
-      <c r="I44" s="71" t="s">
+      <c r="I44" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="J44" s="61">
+      <c r="J44" s="59">
         <f>[1]Graphs!$B$57/1000000</f>
         <v>0.84414999999999996</v>
       </c>
-      <c r="K44" s="61">
+      <c r="K44" s="59">
         <f>[1]Graphs!$C$57/1000000</f>
         <v>0.160411</v>
       </c>
-      <c r="L44" s="61">
+      <c r="L44" s="59">
         <f>E89</f>
         <v>0</v>
       </c>
-      <c r="M44" s="61">
+      <c r="M44" s="59">
         <f>$B$8</f>
         <v>1.0289999999999999</v>
       </c>
@@ -16488,7 +15571,7 @@
         <f>K44/(J44+K44)</f>
         <v>0.15968268726339166</v>
       </c>
-      <c r="P44" s="59">
+      <c r="P44" s="57">
         <f>[1]Graphs!$D$57/([1]Graphs!$B$57+[1]Graphs!$C$57+[1]Graphs!$D$57)</f>
         <v>0</v>
       </c>
@@ -16498,49 +15581,49 @@
       </c>
     </row>
     <row r="45" spans="1:21" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="67" t="s">
+      <c r="A45" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="86">
+      <c r="B45" s="84">
         <f>[1]Summary_legal_compliance!$C$32</f>
         <v>2</v>
       </c>
-      <c r="C45" s="84">
+      <c r="C45" s="82">
         <f>[1]Summary_legal_compliance!$C$31</f>
         <v>2</v>
       </c>
-      <c r="D45" s="85">
+      <c r="D45" s="83">
         <f>[1]Summary_legal_compliance!$D$31</f>
         <v>100</v>
       </c>
-      <c r="E45" s="84">
+      <c r="E45" s="82">
         <f>[1]Summary_legal_compliance!$E$32</f>
         <v>230000</v>
       </c>
-      <c r="F45" s="84">
+      <c r="F45" s="82">
         <f>[1]Summary_legal_compliance!$E$31</f>
         <v>230000</v>
       </c>
-      <c r="G45" s="83">
+      <c r="G45" s="81">
         <f>[1]Summary_legal_compliance!$F$31</f>
         <v>100</v>
       </c>
-      <c r="I45" s="71" t="s">
+      <c r="I45" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="J45" s="61">
+      <c r="J45" s="59">
         <f>[1]Graphs!$B$60/1000000</f>
         <v>0.23</v>
       </c>
-      <c r="K45" s="61">
+      <c r="K45" s="59">
         <f>[1]Graphs!$C$60/1000000</f>
         <v>0</v>
       </c>
-      <c r="L45" s="61">
+      <c r="L45" s="59">
         <f>E93</f>
         <v>0</v>
       </c>
-      <c r="M45" s="61">
+      <c r="M45" s="59">
         <f>$B$8</f>
         <v>1.0289999999999999</v>
       </c>
@@ -16562,10 +15645,10 @@
       </c>
     </row>
     <row r="46" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="82"/>
+      <c r="A46" s="80"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="82"/>
+      <c r="A47" s="80"/>
     </row>
     <row r="48" spans="1:21" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
@@ -16573,7 +15656,7 @@
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A49" s="82"/>
+      <c r="A49" s="80"/>
       <c r="L49" s="12" t="s">
         <v>77</v>
       </c>
@@ -16584,49 +15667,49 @@
     </row>
     <row r="50" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A51" s="162" t="str">
+      <c r="A51" s="152" t="str">
         <f>A1</f>
         <v>Cyprus in 2018</v>
       </c>
       <c r="B51" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="C51" s="160"/>
-      <c r="D51" s="161"/>
+      <c r="C51" s="156"/>
+      <c r="D51" s="157"/>
     </row>
     <row r="52" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="163"/>
-      <c r="B52" s="80" t="s">
+      <c r="A52" s="153"/>
+      <c r="B52" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="80" t="s">
+      <c r="C52" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="D52" s="80" t="s">
+      <c r="D52" s="78" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="163"/>
-      <c r="B53" s="81" t="s">
+      <c r="A53" s="153"/>
+      <c r="B53" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="80" t="s">
+      <c r="C53" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="79" t="s">
+      <c r="D53" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="78" t="s">
+      <c r="F53" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="G53" s="77" t="s">
+      <c r="G53" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="H53" s="76" t="s">
+      <c r="H53" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="I53" s="76" t="s">
+      <c r="I53" s="74" t="s">
         <v>73</v>
       </c>
       <c r="J53" s="1" t="s">
@@ -16637,41 +15720,41 @@
       </c>
     </row>
     <row r="54" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="75" t="s">
+      <c r="A54" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="74">
+      <c r="B54" s="72">
         <f>[1]Graphs!$C$119</f>
         <v>1029000</v>
       </c>
-      <c r="C54" s="73">
+      <c r="C54" s="71">
         <f>[1]Graphs!$C$120</f>
         <v>154061</v>
       </c>
-      <c r="D54" s="72">
+      <c r="D54" s="70">
         <f>[1]Graphs!$B$120</f>
         <v>15</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F54" s="63">
+      <c r="F54" s="61">
         <f>(B54-C54)/1000000</f>
         <v>0.87493900000000002</v>
       </c>
-      <c r="G54" s="63">
+      <c r="G54" s="61">
         <f>C54/1000000</f>
         <v>0.154061</v>
       </c>
-      <c r="H54" s="62">
+      <c r="H54" s="60">
         <f>L43</f>
         <v>0</v>
       </c>
-      <c r="I54" s="61">
+      <c r="I54" s="59">
         <f>$B$8</f>
         <v>1.0289999999999999</v>
       </c>
-      <c r="J54" s="59">
+      <c r="J54" s="57">
         <f>D54/100</f>
         <v>0.15</v>
       </c>
@@ -16681,41 +15764,41 @@
       </c>
     </row>
     <row r="55" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="71" t="s">
+      <c r="A55" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="70">
+      <c r="B55" s="68">
         <f>[1]Graphs!$C$121</f>
         <v>1004561</v>
       </c>
-      <c r="C55" s="69">
+      <c r="C55" s="67">
         <f>[1]Graphs!$C$123</f>
         <v>154061</v>
       </c>
-      <c r="D55" s="68">
+      <c r="D55" s="66">
         <f>[1]Graphs!$B$123</f>
         <v>15.3</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F55" s="63">
+      <c r="F55" s="61">
         <f>(B55-C55)/1000000</f>
         <v>0.85050000000000003</v>
       </c>
-      <c r="G55" s="63">
+      <c r="G55" s="61">
         <f>C55/1000000</f>
         <v>0.154061</v>
       </c>
-      <c r="H55" s="62">
+      <c r="H55" s="60">
         <f>L44</f>
         <v>0</v>
       </c>
-      <c r="I55" s="61">
+      <c r="I55" s="59">
         <f>$B$8</f>
         <v>1.0289999999999999</v>
       </c>
-      <c r="J55" s="59">
+      <c r="J55" s="57">
         <f>D55/100</f>
         <v>0.153</v>
       </c>
@@ -16725,41 +15808,41 @@
       </c>
     </row>
     <row r="56" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="67" t="s">
+      <c r="A56" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="66">
+      <c r="B56" s="64">
         <f>[1]Graphs!$C$124</f>
         <v>230000</v>
       </c>
-      <c r="C56" s="65">
+      <c r="C56" s="63">
         <f>[1]Graphs!$C$126</f>
         <v>0</v>
       </c>
-      <c r="D56" s="64">
+      <c r="D56" s="62">
         <f>[1]Graphs!$B$126</f>
         <v>0</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F56" s="63">
+      <c r="F56" s="61">
         <f>(B56-C56)/1000000</f>
         <v>0.23</v>
       </c>
-      <c r="G56" s="63">
+      <c r="G56" s="61">
         <f>C56/1000000</f>
         <v>0</v>
       </c>
-      <c r="H56" s="62">
+      <c r="H56" s="60">
         <f>L45</f>
         <v>0</v>
       </c>
-      <c r="I56" s="61">
+      <c r="I56" s="59">
         <f>$B$8</f>
         <v>1.0289999999999999</v>
       </c>
-      <c r="J56" s="59">
+      <c r="J56" s="57">
         <f>D56/100</f>
         <v>0</v>
       </c>
@@ -16798,28 +15881,28 @@
     </row>
     <row r="61" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="164" t="s">
+      <c r="A62" s="160" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="165"/>
-      <c r="C62" s="165"/>
-      <c r="D62" s="165"/>
-      <c r="E62" s="166"/>
+      <c r="B62" s="161"/>
+      <c r="C62" s="161"/>
+      <c r="D62" s="161"/>
+      <c r="E62" s="162"/>
     </row>
     <row r="63" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="42"/>
-      <c r="C63" s="60"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="60"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="58"/>
+      <c r="E63" s="58"/>
     </row>
     <row r="64" spans="1:25" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="118" t="s">
+      <c r="C64" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="D64" s="119" t="s">
+      <c r="D64" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="E64" s="120" t="s">
+      <c r="E64" s="118" t="s">
         <v>51</v>
       </c>
       <c r="F64" s="1" t="s">
@@ -16830,22 +15913,23 @@
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A65" s="167" t="s">
+      <c r="A65" s="158" t="s">
         <v>48</v>
       </c>
-      <c r="B65" s="57">
+      <c r="B65" s="55">
         <f>D21</f>
         <v>2014</v>
       </c>
-      <c r="C65" s="56">
+      <c r="C65" s="54">
         <f>[1]Graphs!$B$56/1000000</f>
         <v>0.64649999999999996</v>
       </c>
-      <c r="D65" s="56">
+      <c r="D65" s="54">
         <f>[1]Graphs!$C$56/1000000</f>
         <v>0.34849999999999998</v>
       </c>
-      <c r="E65" s="55">
+      <c r="E65" s="173">
+        <f>[1]Graphs!$E$56/1000000</f>
         <v>0</v>
       </c>
       <c r="F65" s="48">
@@ -16858,20 +15942,21 @@
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A66" s="168"/>
-      <c r="B66" s="54">
+      <c r="A66" s="150"/>
+      <c r="B66" s="53">
         <f>D22</f>
         <v>2016</v>
       </c>
-      <c r="C66" s="53">
+      <c r="C66" s="52">
         <f>[1]Graphs!$B$55/1000000</f>
         <v>0.78</v>
       </c>
-      <c r="D66" s="53">
+      <c r="D66" s="52">
         <f>[1]Graphs!$C$55/1000000</f>
         <v>0.249</v>
       </c>
-      <c r="E66" s="52">
+      <c r="E66" s="174">
+        <f>[1]Graphs!$E$55/1000000</f>
         <v>0</v>
       </c>
       <c r="F66" s="48">
@@ -16884,7 +15969,7 @@
       </c>
     </row>
     <row r="67" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="169"/>
+      <c r="A67" s="151"/>
       <c r="B67" s="51" t="str">
         <f>D23</f>
         <v xml:space="preserve">2018 </v>
@@ -16898,7 +15983,7 @@
         <v>0.16819999999999999</v>
       </c>
       <c r="E67" s="49">
-        <f>[1]Summary_legal_compliance!$E$17/1000000</f>
+        <f>[1]Graphs!$E$54/1000000</f>
         <v>0</v>
       </c>
       <c r="F67" s="48">
@@ -16912,14 +15997,14 @@
     </row>
     <row r="68" spans="1:23" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
-      <c r="B68" s="58"/>
-      <c r="C68" s="118" t="s">
+      <c r="B68" s="56"/>
+      <c r="C68" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="D68" s="119" t="s">
+      <c r="D68" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="E68" s="120" t="s">
+      <c r="E68" s="118" t="s">
         <v>51</v>
       </c>
       <c r="I68" s="10" t="s">
@@ -16927,22 +16012,23 @@
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A69" s="167" t="s">
+      <c r="A69" s="158" t="s">
         <v>45</v>
       </c>
-      <c r="B69" s="57">
+      <c r="B69" s="55">
         <f>D21</f>
         <v>2014</v>
       </c>
-      <c r="C69" s="56">
+      <c r="C69" s="54">
         <f>[1]Graphs!$B$59/1000000</f>
         <v>0.63151000000000002</v>
       </c>
-      <c r="D69" s="56">
+      <c r="D69" s="54">
         <f>[1]Graphs!$C$59/1000000</f>
         <v>0.16756799999999999</v>
       </c>
-      <c r="E69" s="55">
+      <c r="E69" s="173">
+        <f>[1]Graphs!$E$59/1000000</f>
         <v>0</v>
       </c>
       <c r="F69" s="48">
@@ -16955,20 +16041,21 @@
       </c>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A70" s="168"/>
-      <c r="B70" s="54">
+      <c r="A70" s="150"/>
+      <c r="B70" s="53">
         <f>D22</f>
         <v>2016</v>
       </c>
-      <c r="C70" s="53">
+      <c r="C70" s="52">
         <f>[1]Graphs!$B$58/1000000</f>
         <v>0.75255000000000005</v>
       </c>
-      <c r="D70" s="53">
+      <c r="D70" s="52">
         <f>[1]Graphs!$C$58/1000000</f>
         <v>0.240733</v>
       </c>
-      <c r="E70" s="52">
+      <c r="E70" s="174">
+        <f>[1]Graphs!$E$58/1000000</f>
         <v>0</v>
       </c>
       <c r="F70" s="48">
@@ -16981,7 +16068,7 @@
       </c>
     </row>
     <row r="71" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="169"/>
+      <c r="A71" s="151"/>
       <c r="B71" s="51" t="str">
         <f>D23</f>
         <v xml:space="preserve">2018 </v>
@@ -16995,14 +16082,14 @@
         <v>0.160411</v>
       </c>
       <c r="E71" s="49">
-        <f>[1]Summary_legal_compliance!$E$27/1000000</f>
+        <f>[1]Graphs!$E$57/1000000</f>
         <v>0</v>
       </c>
       <c r="F71" s="48">
         <f>IF((C71+D71)&gt;0,C71/(C71+D71),"")</f>
         <v>0.84031731273660826</v>
       </c>
-      <c r="G71" s="59">
+      <c r="G71" s="57">
         <f>D71/(C71+D71+E71)</f>
         <v>0.15968268726339166</v>
       </c>
@@ -17013,14 +16100,14 @@
     </row>
     <row r="72" spans="1:23" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="40"/>
-      <c r="B72" s="58"/>
-      <c r="C72" s="118" t="s">
+      <c r="B72" s="56"/>
+      <c r="C72" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="D72" s="119" t="s">
+      <c r="D72" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="E72" s="120" t="s">
+      <c r="E72" s="118" t="s">
         <v>51</v>
       </c>
       <c r="I72" s="10" t="s">
@@ -17028,22 +16115,23 @@
       </c>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A73" s="167" t="s">
+      <c r="A73" s="158" t="s">
         <v>40</v>
       </c>
-      <c r="B73" s="57">
+      <c r="B73" s="55">
         <f>D21</f>
         <v>2014</v>
       </c>
-      <c r="C73" s="56">
+      <c r="C73" s="54">
         <f>[1]Graphs!$B$62/1000000</f>
         <v>0.16500000000000001</v>
       </c>
-      <c r="D73" s="56">
+      <c r="D73" s="54">
         <f>[1]Graphs!$C$62/1000000</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E73" s="55">
+      <c r="E73" s="173">
+        <f>[1]Graphs!$E$62/1000000</f>
         <v>0</v>
       </c>
       <c r="F73" s="48">
@@ -17056,20 +16144,21 @@
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A74" s="168"/>
-      <c r="B74" s="54">
+      <c r="A74" s="150"/>
+      <c r="B74" s="53">
         <f>D22</f>
         <v>2016</v>
       </c>
-      <c r="C74" s="53">
+      <c r="C74" s="52">
         <f>[1]Graphs!$B$61/1000000</f>
         <v>0.16500000000000001</v>
       </c>
-      <c r="D74" s="53">
+      <c r="D74" s="52">
         <f>[1]Graphs!$C$61/1000000</f>
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="E74" s="52">
+      <c r="E74" s="174">
+        <f>[1]Graphs!$E$61/1000000</f>
         <v>0</v>
       </c>
       <c r="F74" s="48">
@@ -17082,7 +16171,7 @@
       </c>
     </row>
     <row r="75" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="169"/>
+      <c r="A75" s="151"/>
       <c r="B75" s="51" t="str">
         <f>D23</f>
         <v xml:space="preserve">2018 </v>
@@ -17096,7 +16185,7 @@
         <v>0</v>
       </c>
       <c r="E75" s="49">
-        <f>[1]Summary_legal_compliance!$E$40/1000000</f>
+        <f>[1]Graphs!$E$60/1000000</f>
         <v>0</v>
       </c>
       <c r="F75" s="48">
@@ -17149,19 +16238,19 @@
       <c r="E81" s="43"/>
     </row>
     <row r="82" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="116" t="s">
+      <c r="C82" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="D82" s="117" t="s">
+      <c r="D82" s="115" t="s">
         <v>52</v>
       </c>
-      <c r="E82" s="147" t="s">
+      <c r="E82" s="145" t="s">
         <v>51</v>
       </c>
       <c r="F82" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="G82" s="148" t="s">
+      <c r="G82" s="146" t="s">
         <v>42</v>
       </c>
       <c r="I82" s="41" t="s">
@@ -17169,22 +16258,22 @@
       </c>
     </row>
     <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A83" s="170" t="s">
+      <c r="A83" s="147" t="s">
         <v>48</v>
       </c>
-      <c r="B83" s="130">
+      <c r="B83" s="128">
         <f>D21</f>
         <v>2014</v>
       </c>
-      <c r="C83" s="134">
+      <c r="C83" s="132">
         <f>G83-D83</f>
         <v>0.75434999999999997</v>
       </c>
-      <c r="D83" s="140">
+      <c r="D83" s="138">
         <f>[1]Graphs!$G$120/1000000</f>
         <v>0.24065</v>
       </c>
-      <c r="E83" s="137">
+      <c r="E83" s="135">
         <f t="shared" ref="E83:E93" si="0">E65</f>
         <v>0</v>
       </c>
@@ -17192,7 +16281,7 @@
         <f>IF(D83&lt;&gt;0,D83/G83,"")</f>
         <v>0.24185929648241206</v>
       </c>
-      <c r="G83" s="140">
+      <c r="G83" s="138">
         <f>[1]Graphs!$G$119/1000000</f>
         <v>0.995</v>
       </c>
@@ -17202,20 +16291,20 @@
       </c>
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A84" s="171"/>
-      <c r="B84" s="131">
+      <c r="A84" s="148"/>
+      <c r="B84" s="129">
         <f>D22</f>
         <v>2016</v>
       </c>
-      <c r="C84" s="135">
+      <c r="C84" s="133">
         <f>G84-D84</f>
         <v>0.85400599999999993</v>
       </c>
-      <c r="D84" s="141">
+      <c r="D84" s="139">
         <f>[1]Graphs!$E$120/1000000</f>
         <v>0.17499400000000001</v>
       </c>
-      <c r="E84" s="138">
+      <c r="E84" s="136">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17223,7 +16312,7 @@
         <f>IF(D84&lt;&gt;0,D84/G84,"")</f>
         <v>0.17006219630709429</v>
       </c>
-      <c r="G84" s="141">
+      <c r="G84" s="139">
         <f>[1]Graphs!$E$119/1000000</f>
         <v>1.0289999999999999</v>
       </c>
@@ -17237,20 +16326,20 @@
       </c>
     </row>
     <row r="85" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="172"/>
-      <c r="B85" s="132" t="str">
+      <c r="A85" s="149"/>
+      <c r="B85" s="130" t="str">
         <f>D23</f>
         <v xml:space="preserve">2018 </v>
       </c>
-      <c r="C85" s="136">
+      <c r="C85" s="134">
         <f>G85-D85</f>
         <v>0.87493899999999991</v>
       </c>
-      <c r="D85" s="142">
+      <c r="D85" s="140">
         <f>[1]Graphs!$C$120/1000000</f>
         <v>0.154061</v>
       </c>
-      <c r="E85" s="139">
+      <c r="E85" s="137">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17258,7 +16347,7 @@
         <f>IF(D85&lt;&gt;0,D85/G85,"")</f>
         <v>0.14971914480077747</v>
       </c>
-      <c r="G85" s="142">
+      <c r="G85" s="140">
         <f>[1]Graphs!$C$119/1000000</f>
         <v>1.0289999999999999</v>
       </c>
@@ -17273,19 +16362,19 @@
     </row>
     <row r="86" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="40"/>
-      <c r="B86" s="121"/>
-      <c r="C86" s="122" t="s">
+      <c r="B86" s="119"/>
+      <c r="C86" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="D86" s="123" t="s">
+      <c r="D86" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="E86" s="146" t="str">
+      <c r="E86" s="144" t="str">
         <f t="shared" si="0"/>
         <v>Pending</v>
       </c>
       <c r="F86" s="36"/>
-      <c r="G86" s="148" t="s">
+      <c r="G86" s="146" t="s">
         <v>42</v>
       </c>
       <c r="I86" s="10" t="s">
@@ -17293,22 +16382,22 @@
       </c>
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="168" t="s">
+      <c r="A87" s="150" t="s">
         <v>45</v>
       </c>
-      <c r="B87" s="133">
+      <c r="B87" s="131">
         <f>D21</f>
         <v>2014</v>
       </c>
-      <c r="C87" s="143">
+      <c r="C87" s="141">
         <f>G87-D87</f>
         <v>0.73692799999999992</v>
       </c>
-      <c r="D87" s="140">
+      <c r="D87" s="138">
         <f>[1]Graphs!$G$123/1000000</f>
         <v>6.2149999999999997E-2</v>
       </c>
-      <c r="E87" s="137">
+      <c r="E87" s="135">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17316,7 +16405,7 @@
         <f>IF(D87&lt;&gt;0,D87/G87,"")</f>
         <v>7.7777138151719855E-2</v>
       </c>
-      <c r="G87" s="140">
+      <c r="G87" s="138">
         <f>[1]Graphs!$G$121/1000000</f>
         <v>0.79907799999999995</v>
       </c>
@@ -17326,20 +16415,20 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="168"/>
+      <c r="A88" s="150"/>
       <c r="B88" s="38">
         <f>D22</f>
         <v>2016</v>
       </c>
-      <c r="C88" s="144">
+      <c r="C88" s="142">
         <f>G88-D88</f>
         <v>0.81988900000000009</v>
       </c>
-      <c r="D88" s="141">
+      <c r="D88" s="139">
         <f>[1]Graphs!$E$123/1000000</f>
         <v>0.17339399999999999</v>
       </c>
-      <c r="E88" s="138">
+      <c r="E88" s="136">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17347,7 +16436,7 @@
         <f>IF(D88&lt;&gt;0,D88/G88,"")</f>
         <v>0.17456656360775327</v>
       </c>
-      <c r="G88" s="141">
+      <c r="G88" s="139">
         <f>[1]Graphs!$E$121/1000000</f>
         <v>0.99328300000000003</v>
       </c>
@@ -17361,20 +16450,20 @@
       </c>
     </row>
     <row r="89" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="169"/>
+      <c r="A89" s="151"/>
       <c r="B89" s="37" t="str">
         <f>D23</f>
         <v xml:space="preserve">2018 </v>
       </c>
-      <c r="C89" s="145">
+      <c r="C89" s="143">
         <f>G89-D89</f>
         <v>0.85050000000000003</v>
       </c>
-      <c r="D89" s="142">
+      <c r="D89" s="140">
         <f>[1]Graphs!$C$123/1000000</f>
         <v>0.154061</v>
       </c>
-      <c r="E89" s="139">
+      <c r="E89" s="137">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17382,7 +16471,7 @@
         <f>IF(D89&lt;&gt;0,D89/G89,"")</f>
         <v>0.15336151811587351</v>
       </c>
-      <c r="G89" s="142">
+      <c r="G89" s="140">
         <f>[1]Graphs!$C$121/1000000</f>
         <v>1.004561</v>
       </c>
@@ -17398,18 +16487,18 @@
     <row r="90" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="40"/>
       <c r="B90" s="39"/>
-      <c r="C90" s="122" t="s">
+      <c r="C90" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="D90" s="123" t="s">
+      <c r="D90" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="E90" s="146" t="str">
+      <c r="E90" s="144" t="str">
         <f t="shared" si="0"/>
         <v>Pending</v>
       </c>
       <c r="F90" s="36"/>
-      <c r="G90" s="148" t="s">
+      <c r="G90" s="146" t="s">
         <v>42</v>
       </c>
       <c r="I90" s="10" t="s">
@@ -17417,22 +16506,22 @@
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A91" s="168" t="s">
+      <c r="A91" s="150" t="s">
         <v>40</v>
       </c>
       <c r="B91" s="38">
         <f>D21</f>
         <v>2014</v>
       </c>
-      <c r="C91" s="143">
+      <c r="C91" s="141">
         <f>G91-D91</f>
         <v>0.23</v>
       </c>
-      <c r="D91" s="140">
+      <c r="D91" s="138">
         <f>[1]Graphs!$G$126/1000000</f>
         <v>0</v>
       </c>
-      <c r="E91" s="137">
+      <c r="E91" s="135">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17440,7 +16529,7 @@
         <f>IF(D91&lt;&gt;0,D91/G91,"")</f>
         <v/>
       </c>
-      <c r="G91" s="140">
+      <c r="G91" s="138">
         <f>[1]Graphs!$G$124/1000000</f>
         <v>0.23</v>
       </c>
@@ -17450,20 +16539,20 @@
       </c>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A92" s="168"/>
+      <c r="A92" s="150"/>
       <c r="B92" s="38">
         <f>D22</f>
         <v>2016</v>
       </c>
-      <c r="C92" s="144">
+      <c r="C92" s="142">
         <f>G92-D92</f>
         <v>0.22869999999999999</v>
       </c>
-      <c r="D92" s="141">
+      <c r="D92" s="139">
         <f>[1]Graphs!$E$126/1000000</f>
         <v>0</v>
       </c>
-      <c r="E92" s="138">
+      <c r="E92" s="136">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17471,7 +16560,7 @@
         <f>IF(D92&lt;&gt;0,D92/G92,"")</f>
         <v/>
       </c>
-      <c r="G92" s="141">
+      <c r="G92" s="139">
         <f>[1]Graphs!$E$124/1000000</f>
         <v>0.22869999999999999</v>
       </c>
@@ -17485,20 +16574,20 @@
       </c>
     </row>
     <row r="93" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="169"/>
+      <c r="A93" s="151"/>
       <c r="B93" s="37" t="str">
         <f>D23</f>
         <v xml:space="preserve">2018 </v>
       </c>
-      <c r="C93" s="145">
+      <c r="C93" s="143">
         <f>G93-D93</f>
         <v>0.23</v>
       </c>
-      <c r="D93" s="142">
+      <c r="D93" s="140">
         <f>[1]Graphs!$C$126/1000000</f>
         <v>0</v>
       </c>
-      <c r="E93" s="139">
+      <c r="E93" s="137">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17506,7 +16595,7 @@
         <f>IF(D93&lt;&gt;0,D93/G93,"")</f>
         <v/>
       </c>
-      <c r="G93" s="142">
+      <c r="G93" s="140">
         <f>[1]Graphs!$C$124/1000000</f>
         <v>0.23</v>
       </c>
@@ -17573,21 +16662,21 @@
       <c r="T101" s="35"/>
     </row>
     <row r="102" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="114" t="str">
+      <c r="A102" s="112" t="str">
         <f>[1]Graphs!$A$73</f>
         <v>Summary installation in place</v>
       </c>
-      <c r="B102" s="124">
+      <c r="B102" s="122">
         <f>D22</f>
         <v>2016</v>
       </c>
-      <c r="C102" s="124" t="str">
+      <c r="C102" s="122" t="str">
         <f>D23</f>
         <v xml:space="preserve">2018 </v>
       </c>
     </row>
     <row r="103" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A103" s="125" t="s">
+      <c r="A103" s="123" t="s">
         <v>119</v>
       </c>
       <c r="B103" s="6">
@@ -17603,7 +16692,7 @@
       </c>
     </row>
     <row r="104" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A104" s="125" t="s">
+      <c r="A104" s="123" t="s">
         <v>120</v>
       </c>
       <c r="B104" s="6">
@@ -17616,7 +16705,7 @@
       </c>
     </row>
     <row r="105" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A105" s="125" t="s">
+      <c r="A105" s="123" t="s">
         <v>121</v>
       </c>
       <c r="B105" s="6">
@@ -17629,7 +16718,7 @@
       </c>
     </row>
     <row r="106" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A106" s="125" t="s">
+      <c r="A106" s="123" t="s">
         <v>122</v>
       </c>
       <c r="B106" s="6">
@@ -17642,7 +16731,7 @@
       </c>
     </row>
     <row r="107" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A107" s="125" t="s">
+      <c r="A107" s="123" t="s">
         <v>123</v>
       </c>
       <c r="B107" s="6">
@@ -17655,7 +16744,7 @@
       </c>
     </row>
     <row r="108" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A108" s="125" t="s">
+      <c r="A108" s="123" t="s">
         <v>124</v>
       </c>
       <c r="B108" s="6">
@@ -17684,27 +16773,27 @@
     </row>
     <row r="119" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="6"/>
-      <c r="B119" s="113">
+      <c r="B119" s="111">
         <f>D21</f>
         <v>2014</v>
       </c>
-      <c r="C119" s="113">
+      <c r="C119" s="111">
         <f>D22</f>
         <v>2016</v>
       </c>
-      <c r="D119" s="113" t="str">
+      <c r="D119" s="111" t="str">
         <f>D23</f>
         <v xml:space="preserve">2018 </v>
       </c>
-      <c r="E119" s="113">
+      <c r="E119" s="111">
         <f>B119</f>
         <v>2014</v>
       </c>
-      <c r="F119" s="113">
+      <c r="F119" s="111">
         <f>C119</f>
         <v>2016</v>
       </c>
-      <c r="G119" s="113" t="str">
+      <c r="G119" s="111" t="str">
         <f>D119</f>
         <v xml:space="preserve">2018 </v>
       </c>
@@ -17754,11 +16843,11 @@
         <f>[1]Graphs!$B$26</f>
         <v>6900</v>
       </c>
-      <c r="E121" s="112">
+      <c r="E121" s="110">
         <f>IF(E120&lt;0.0005,"",E120)</f>
         <v>0.22904659970360614</v>
       </c>
-      <c r="F121" s="112">
+      <c r="F121" s="110">
         <f>IF(F120&lt;0.0005,"",F120)</f>
         <v>0.21773758099352053</v>
       </c>
@@ -17836,18 +16925,18 @@
       </c>
     </row>
     <row r="126" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="114" t="s">
+      <c r="A126" s="112" t="s">
         <v>114</v>
       </c>
-      <c r="B126" s="115">
+      <c r="B126" s="113">
         <f>SUM(B120:B125)</f>
         <v>6073</v>
       </c>
-      <c r="C126" s="115">
+      <c r="C126" s="113">
         <f>SUM(C120:C125)</f>
         <v>7408</v>
       </c>
-      <c r="D126" s="115">
+      <c r="D126" s="113">
         <f>SUM(D120:D125)</f>
         <v>8177</v>
       </c>
@@ -17863,21 +16952,21 @@
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="154" t="str">
+      <c r="A142" s="163" t="str">
         <f>A1</f>
         <v>Cyprus in 2018</v>
       </c>
-      <c r="B142" s="156" t="s">
+      <c r="B142" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="C142" s="157"/>
-      <c r="D142" s="156" t="s">
+      <c r="C142" s="166"/>
+      <c r="D142" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="E142" s="157"/>
+      <c r="E142" s="166"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" s="155"/>
+      <c r="A143" s="164"/>
       <c r="B143" s="34" t="s">
         <v>35</v>
       </c>
@@ -18050,31 +17139,31 @@
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A155" s="158" t="str">
+      <c r="A155" s="167" t="str">
         <f>A1</f>
         <v>Cyprus in 2018</v>
       </c>
-      <c r="B155" s="158"/>
-      <c r="C155" s="158"/>
-      <c r="D155" s="149" t="s">
+      <c r="B155" s="167"/>
+      <c r="C155" s="167"/>
+      <c r="D155" s="168" t="s">
         <v>8</v>
       </c>
-      <c r="E155" s="149"/>
-      <c r="F155" s="149" t="s">
+      <c r="E155" s="168"/>
+      <c r="F155" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="G155" s="149"/>
-      <c r="H155" s="149"/>
-      <c r="I155" s="149" t="s">
+      <c r="G155" s="168"/>
+      <c r="H155" s="168"/>
+      <c r="I155" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="J155" s="149"/>
-      <c r="K155" s="149"/>
-      <c r="L155" s="149" t="s">
+      <c r="J155" s="168"/>
+      <c r="K155" s="168"/>
+      <c r="L155" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="M155" s="149"/>
-      <c r="N155" s="149"/>
+      <c r="M155" s="168"/>
+      <c r="N155" s="168"/>
     </row>
     <row r="156" spans="1:14" ht="91.5" x14ac:dyDescent="0.2">
       <c r="A156" s="9" t="s">
@@ -20678,33 +19767,33 @@
       </c>
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A210" s="152" t="s">
+      <c r="A210" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="B210" s="152" t="s">
+      <c r="B210" s="171" t="s">
         <v>10</v>
       </c>
-      <c r="C210" s="152" t="s">
+      <c r="C210" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="D210" s="149" t="s">
+      <c r="D210" s="168" t="s">
         <v>8</v>
       </c>
-      <c r="E210" s="149"/>
-      <c r="F210" s="149"/>
-      <c r="G210" s="153" t="s">
+      <c r="E210" s="168"/>
+      <c r="F210" s="168"/>
+      <c r="G210" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="H210" s="153"/>
-      <c r="I210" s="153"/>
-      <c r="J210" s="150" t="s">
+      <c r="H210" s="172"/>
+      <c r="I210" s="172"/>
+      <c r="J210" s="169" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="211" spans="1:10" ht="69.75" x14ac:dyDescent="0.2">
-      <c r="A211" s="152"/>
-      <c r="B211" s="152"/>
-      <c r="C211" s="152"/>
+      <c r="A211" s="171"/>
+      <c r="B211" s="171"/>
+      <c r="C211" s="171"/>
       <c r="D211" s="9" t="s">
         <v>5</v>
       </c>
@@ -20723,7 +19812,7 @@
       <c r="I211" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J211" s="151"/>
+      <c r="J211" s="170"/>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" s="6" t="str">
@@ -26061,23 +25150,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A87:A89"/>
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="A155:C155"/>
-    <mergeCell ref="D155:E155"/>
     <mergeCell ref="F155:H155"/>
     <mergeCell ref="I155:K155"/>
     <mergeCell ref="J210:J211"/>
@@ -26087,6 +25159,23 @@
     <mergeCell ref="C210:C211"/>
     <mergeCell ref="D210:F210"/>
     <mergeCell ref="G210:I210"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="A155:C155"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A73:A75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>